<commit_message>
skeleton plus all ponds
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_Filtered_Data_with_real_length.xlsx
@@ -603,7 +603,9 @@
       <c r="S2" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>38.4633237865796</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -673,7 +675,9 @@
       <c r="S3" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>28.90841249553062</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -743,7 +747,9 @@
       <c r="S4" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>39.58479455863773</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -813,7 +819,9 @@
       <c r="S5" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>25.08731753405586</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -883,7 +891,9 @@
       <c r="S6" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>22.56153606765636</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -953,7 +963,9 @@
       <c r="S7" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>25.0324391292011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1023,7 +1035,9 @@
       <c r="S8" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T8" t="inlineStr"/>
+      <c r="T8" t="n">
+        <v>35.92035186635304</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1093,7 +1107,9 @@
       <c r="S9" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T9" t="inlineStr"/>
+      <c r="T9" t="n">
+        <v>33.25101619038021</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1163,7 +1179,9 @@
       <c r="S10" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T10" t="inlineStr"/>
+      <c r="T10" t="n">
+        <v>25.66259612043985</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1233,7 +1251,9 @@
       <c r="S11" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T11" t="inlineStr"/>
+      <c r="T11" t="n">
+        <v>29.99930527034374</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1303,7 +1323,9 @@
       <c r="S12" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T12" t="inlineStr"/>
+      <c r="T12" t="n">
+        <v>36.77899511119482</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1373,7 +1395,9 @@
       <c r="S13" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T13" t="inlineStr"/>
+      <c r="T13" t="n">
+        <v>29.85513969827502</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1443,7 +1467,9 @@
       <c r="S14" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>30.6454209858543</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1513,7 +1539,9 @@
       <c r="S15" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T15" t="inlineStr"/>
+      <c r="T15" t="n">
+        <v>33.6003689178345</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1583,7 +1611,9 @@
       <c r="S16" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T16" t="inlineStr"/>
+      <c r="T16" t="n">
+        <v>14.88120358976283</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1653,7 +1683,9 @@
       <c r="S17" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>26.3800861266348</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1723,7 +1755,9 @@
       <c r="S18" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>35.82629067865172</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1793,7 +1827,9 @@
       <c r="S19" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T19" t="inlineStr"/>
+      <c r="T19" t="n">
+        <v>29.95368238432675</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1863,7 +1899,9 @@
       <c r="S20" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T20" t="inlineStr"/>
+      <c r="T20" t="n">
+        <v>40.83064690332304</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1933,7 +1971,9 @@
       <c r="S21" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T21" t="inlineStr"/>
+      <c r="T21" t="n">
+        <v>31.81792909839421</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2003,7 +2043,9 @@
       <c r="S22" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T22" t="inlineStr"/>
+      <c r="T22" t="n">
+        <v>39.09854501863349</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2073,7 +2115,9 @@
       <c r="S23" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T23" t="inlineStr"/>
+      <c r="T23" t="n">
+        <v>32.60443710561533</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2143,7 +2187,9 @@
       <c r="S24" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T24" t="inlineStr"/>
+      <c r="T24" t="n">
+        <v>33.74812852721058</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2213,7 +2259,9 @@
       <c r="S25" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T25" t="inlineStr"/>
+      <c r="T25" t="n">
+        <v>13.4375697239241</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2283,7 +2331,9 @@
       <c r="S26" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T26" t="inlineStr"/>
+      <c r="T26" t="n">
+        <v>40.86265353499343</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2353,7 +2403,9 @@
       <c r="S27" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T27" t="inlineStr"/>
+      <c r="T27" t="n">
+        <v>26.71088638279051</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2913,7 +2965,9 @@
       <c r="S35" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T35" t="inlineStr"/>
+      <c r="T35" t="n">
+        <v>29.66716495857016</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2983,7 +3037,9 @@
       <c r="S36" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T36" t="inlineStr"/>
+      <c r="T36" t="n">
+        <v>38.57159027353561</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3053,7 +3109,9 @@
       <c r="S37" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T37" t="inlineStr"/>
+      <c r="T37" t="n">
+        <v>25.38946462654251</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3123,7 +3181,9 @@
       <c r="S38" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T38" t="inlineStr"/>
+      <c r="T38" t="n">
+        <v>41.82014928176122</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3193,7 +3253,9 @@
       <c r="S39" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T39" t="inlineStr"/>
+      <c r="T39" t="n">
+        <v>40.6362236076846</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3263,7 +3325,9 @@
       <c r="S40" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T40" t="inlineStr"/>
+      <c r="T40" t="n">
+        <v>24.59366620671134</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3333,7 +3397,9 @@
       <c r="S41" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T41" t="inlineStr"/>
+      <c r="T41" t="n">
+        <v>38.88348622483628</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3403,7 +3469,9 @@
       <c r="S42" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T42" t="inlineStr"/>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3473,7 +3541,9 @@
       <c r="S43" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T43" t="inlineStr"/>
+      <c r="T43" t="n">
+        <v>37.25549928137975</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3543,7 +3613,9 @@
       <c r="S44" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T44" t="inlineStr"/>
+      <c r="T44" t="n">
+        <v>28.29811256526354</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3613,7 +3685,9 @@
       <c r="S45" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T45" t="inlineStr"/>
+      <c r="T45" t="n">
+        <v>31.1195526044811</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3683,7 +3757,9 @@
       <c r="S46" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T46" t="inlineStr"/>
+      <c r="T46" t="n">
+        <v>31.1195526044811</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3753,7 +3829,9 @@
       <c r="S47" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T47" t="inlineStr"/>
+      <c r="T47" t="n">
+        <v>27.31090890939526</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3823,7 +3901,9 @@
       <c r="S48" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T48" t="inlineStr"/>
+      <c r="T48" t="n">
+        <v>35.69938430494975</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3893,7 +3973,9 @@
       <c r="S49" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T49" t="inlineStr"/>
+      <c r="T49" t="n">
+        <v>35.66872639569743</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3963,7 +4045,9 @@
       <c r="S50" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T50" t="inlineStr"/>
+      <c r="T50" t="n">
+        <v>37.80206187604055</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4033,7 +4117,9 @@
       <c r="S51" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T51" t="inlineStr"/>
+      <c r="T51" t="n">
+        <v>27.27328331517984</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4103,7 +4189,9 @@
       <c r="S52" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T52" t="inlineStr"/>
+      <c r="T52" t="n">
+        <v>32.61034635295254</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -4173,7 +4261,9 @@
       <c r="S53" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T53" t="inlineStr"/>
+      <c r="T53" t="n">
+        <v>33.05552903157839</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4243,7 +4333,9 @@
       <c r="S54" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T54" t="inlineStr"/>
+      <c r="T54" t="n">
+        <v>32.94869791238239</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4313,7 +4405,9 @@
       <c r="S55" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T55" t="inlineStr"/>
+      <c r="T55" t="n">
+        <v>37.9223596053432</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4383,7 +4477,9 @@
       <c r="S56" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T56" t="inlineStr"/>
+      <c r="T56" t="n">
+        <v>22.77184097144083</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4453,7 +4549,9 @@
       <c r="S57" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T57" t="inlineStr"/>
+      <c r="T57" t="n">
+        <v>29.37688020749116</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4523,7 +4621,9 @@
       <c r="S58" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T58" t="inlineStr"/>
+      <c r="T58" t="n">
+        <v>41.04519345454099</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4593,7 +4693,9 @@
       <c r="S59" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T59" t="inlineStr"/>
+      <c r="T59" t="n">
+        <v>41.04519345454099</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4663,7 +4765,9 @@
       <c r="S60" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T60" t="inlineStr"/>
+      <c r="T60" t="n">
+        <v>22.77184097144083</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4733,7 +4837,9 @@
       <c r="S61" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T61" t="inlineStr"/>
+      <c r="T61" t="n">
+        <v>5.932218397323056</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4803,7 +4909,9 @@
       <c r="S62" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T62" t="inlineStr"/>
+      <c r="T62" t="n">
+        <v>36.2494911237218</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4873,7 +4981,9 @@
       <c r="S63" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T63" t="inlineStr"/>
+      <c r="T63" t="n">
+        <v>22.68334623615863</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4943,7 +5053,9 @@
       <c r="S64" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T64" t="inlineStr"/>
+      <c r="T64" t="n">
+        <v>21.4270352236767</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -5013,7 +5125,9 @@
       <c r="S65" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T65" t="inlineStr"/>
+      <c r="T65" t="n">
+        <v>44.6018161614268</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5083,7 +5197,9 @@
       <c r="S66" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T66" t="inlineStr"/>
+      <c r="T66" t="n">
+        <v>32.86013969936226</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -5153,7 +5269,9 @@
       <c r="S67" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T67" t="inlineStr"/>
+      <c r="T67" t="n">
+        <v>23.94292818163721</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -5223,7 +5341,9 @@
       <c r="S68" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T68" t="inlineStr"/>
+      <c r="T68" t="n">
+        <v>32.07007888525862</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -5293,7 +5413,9 @@
       <c r="S69" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T69" t="inlineStr"/>
+      <c r="T69" t="n">
+        <v>40.77401073165723</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5363,7 +5485,9 @@
       <c r="S70" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T70" t="inlineStr"/>
+      <c r="T70" t="n">
+        <v>22.54608821295353</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -5433,7 +5557,9 @@
       <c r="S71" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T71" t="inlineStr"/>
+      <c r="T71" t="n">
+        <v>30.66559632295112</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -5503,7 +5629,9 @@
       <c r="S72" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T72" t="inlineStr"/>
+      <c r="T72" t="n">
+        <v>36.78868115922425</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -5573,7 +5701,9 @@
       <c r="S73" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T73" t="inlineStr"/>
+      <c r="T73" t="n">
+        <v>35.61726580577677</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -5643,7 +5773,9 @@
       <c r="S74" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T74" t="inlineStr"/>
+      <c r="T74" t="n">
+        <v>35.98502691473605</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5713,7 +5845,9 @@
       <c r="S75" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T75" t="inlineStr"/>
+      <c r="T75" t="n">
+        <v>37.28961843891066</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5783,7 +5917,9 @@
       <c r="S76" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T76" t="inlineStr"/>
+      <c r="T76" t="n">
+        <v>37.15197798132769</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5853,7 +5989,9 @@
       <c r="S77" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T77" t="inlineStr"/>
+      <c r="T77" t="n">
+        <v>27.89060114459023</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5923,7 +6061,9 @@
       <c r="S78" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T78" t="inlineStr"/>
+      <c r="T78" t="n">
+        <v>26.24450967504827</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -5993,7 +6133,9 @@
       <c r="S79" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T79" t="inlineStr"/>
+      <c r="T79" t="n">
+        <v>32.27511536018605</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -6063,7 +6205,9 @@
       <c r="S80" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T80" t="inlineStr"/>
+      <c r="T80" t="n">
+        <v>33.05232270520634</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -6133,7 +6277,9 @@
       <c r="S81" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T81" t="inlineStr"/>
+      <c r="T81" t="n">
+        <v>37.91380773744524</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -6203,7 +6349,9 @@
       <c r="S82" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T82" t="inlineStr"/>
+      <c r="T82" t="n">
+        <v>21.69298224001026</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -6273,7 +6421,9 @@
       <c r="S83" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T83" t="inlineStr"/>
+      <c r="T83" t="n">
+        <v>38.9287987021165</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -6343,7 +6493,9 @@
       <c r="S84" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T84" t="inlineStr"/>
+      <c r="T84" t="n">
+        <v>29.76221372731837</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -6413,7 +6565,9 @@
       <c r="S85" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T85" t="inlineStr"/>
+      <c r="T85" t="n">
+        <v>41.09995843088404</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -6483,7 +6637,9 @@
       <c r="S86" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T86" t="inlineStr"/>
+      <c r="T86" t="n">
+        <v>33.02120064349632</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -6553,7 +6709,9 @@
       <c r="S87" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T87" t="inlineStr"/>
+      <c r="T87" t="n">
+        <v>29.65910939016912</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -6623,7 +6781,9 @@
       <c r="S88" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T88" t="inlineStr"/>
+      <c r="T88" t="n">
+        <v>30.11506256205754</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6693,7 +6853,9 @@
       <c r="S89" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T89" t="inlineStr"/>
+      <c r="T89" t="n">
+        <v>37.16291925265281</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6763,7 +6925,9 @@
       <c r="S90" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T90" t="inlineStr"/>
+      <c r="T90" t="n">
+        <v>39.37405917893729</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -6833,7 +6997,9 @@
       <c r="S91" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T91" t="inlineStr"/>
+      <c r="T91" t="n">
+        <v>28.15365666098232</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -6903,7 +7069,9 @@
       <c r="S92" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T92" t="inlineStr"/>
+      <c r="T92" t="n">
+        <v>36.02324033101383</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -6973,7 +7141,9 @@
       <c r="S93" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T93" t="inlineStr"/>
+      <c r="T93" t="n">
+        <v>36.02324033101383</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -7043,7 +7213,9 @@
       <c r="S94" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T94" t="inlineStr"/>
+      <c r="T94" t="n">
+        <v>42.04655497189034</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -7113,7 +7285,9 @@
       <c r="S95" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T95" t="inlineStr"/>
+      <c r="T95" t="n">
+        <v>42.04655497189034</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -7183,7 +7357,9 @@
       <c r="S96" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T96" t="inlineStr"/>
+      <c r="T96" t="n">
+        <v>28.55569977185347</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -7253,7 +7429,9 @@
       <c r="S97" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T97" t="inlineStr"/>
+      <c r="T97" t="n">
+        <v>25.08352199801356</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -7323,7 +7501,9 @@
       <c r="S98" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T98" t="inlineStr"/>
+      <c r="T98" t="n">
+        <v>32.10890210100942</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -7393,7 +7573,9 @@
       <c r="S99" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T99" t="inlineStr"/>
+      <c r="T99" t="n">
+        <v>35.24787868406799</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -7743,7 +7925,9 @@
       <c r="S104" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T104" t="inlineStr"/>
+      <c r="T104" t="n">
+        <v>41.69927347902058</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -7813,7 +7997,9 @@
       <c r="S105" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T105" t="inlineStr"/>
+      <c r="T105" t="n">
+        <v>33.65194007901309</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -8163,7 +8349,9 @@
       <c r="S110" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T110" t="inlineStr"/>
+      <c r="T110" t="n">
+        <v>27.55312813747785</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8233,7 +8421,9 @@
       <c r="S111" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T111" t="inlineStr"/>
+      <c r="T111" t="n">
+        <v>30.50735045245302</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8303,7 +8493,9 @@
       <c r="S112" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T112" t="inlineStr"/>
+      <c r="T112" t="n">
+        <v>30.35488466805121</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -8373,7 +8565,9 @@
       <c r="S113" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T113" t="inlineStr"/>
+      <c r="T113" t="n">
+        <v>36.95209972476533</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8443,7 +8637,9 @@
       <c r="S114" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T114" t="inlineStr"/>
+      <c r="T114" t="n">
+        <v>38.28643206145068</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8513,7 +8709,9 @@
       <c r="S115" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T115" t="inlineStr"/>
+      <c r="T115" t="n">
+        <v>31.30521510351421</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -8583,7 +8781,9 @@
       <c r="S116" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T116" t="inlineStr"/>
+      <c r="T116" t="n">
+        <v>31.30521510351421</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -8653,7 +8853,9 @@
       <c r="S117" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T117" t="inlineStr"/>
+      <c r="T117" t="n">
+        <v>39.32170888326723</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8723,7 +8925,9 @@
       <c r="S118" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T118" t="inlineStr"/>
+      <c r="T118" t="n">
+        <v>25.9641771671566</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -8793,7 +8997,9 @@
       <c r="S119" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T119" t="inlineStr"/>
+      <c r="T119" t="n">
+        <v>47.34216650991087</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -8863,7 +9069,9 @@
       <c r="S120" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T120" t="inlineStr"/>
+      <c r="T120" t="n">
+        <v>27.33787097916291</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -8933,7 +9141,9 @@
       <c r="S121" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T121" t="inlineStr"/>
+      <c r="T121" t="n">
+        <v>30.76737122817728</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -9003,7 +9213,9 @@
       <c r="S122" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T122" t="inlineStr"/>
+      <c r="T122" t="n">
+        <v>35.66874734664732</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -9073,7 +9285,9 @@
       <c r="S123" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T123" t="inlineStr"/>
+      <c r="T123" t="n">
+        <v>17.70668971733859</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -9143,7 +9357,9 @@
       <c r="S124" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T124" t="inlineStr"/>
+      <c r="T124" t="n">
+        <v>33.17591760582172</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -9213,7 +9429,9 @@
       <c r="S125" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T125" t="inlineStr"/>
+      <c r="T125" t="n">
+        <v>43.44318443566831</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -9283,7 +9501,9 @@
       <c r="S126" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T126" t="inlineStr"/>
+      <c r="T126" t="n">
+        <v>30.54452112120853</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -9353,7 +9573,9 @@
       <c r="S127" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T127" t="inlineStr"/>
+      <c r="T127" t="n">
+        <v>34.7428440738251</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -9423,7 +9645,9 @@
       <c r="S128" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T128" t="inlineStr"/>
+      <c r="T128" t="n">
+        <v>33.38487950600774</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -9493,7 +9717,9 @@
       <c r="S129" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T129" t="inlineStr"/>
+      <c r="T129" t="n">
+        <v>31.42351786084434</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -9563,7 +9789,9 @@
       <c r="S130" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T130" t="inlineStr"/>
+      <c r="T130" t="n">
+        <v>44.99084352523037</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -10123,9 +10351,7 @@
       <c r="S138" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T138" t="n">
-        <v>26.08612515129033</v>
-      </c>
+      <c r="T138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -10195,9 +10421,7 @@
       <c r="S139" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T139" t="n">
-        <v>23.93050460653195</v>
-      </c>
+      <c r="T139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -10337,9 +10561,7 @@
       <c r="S141" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T141" t="n">
-        <v>27.49219583602434</v>
-      </c>
+      <c r="T141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -10409,9 +10631,7 @@
       <c r="S142" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T142" t="n">
-        <v>19.61295836078678</v>
-      </c>
+      <c r="T142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -10551,9 +10771,7 @@
       <c r="S144" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T144" t="n">
-        <v>22.19111224848443</v>
-      </c>
+      <c r="T144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -10763,9 +10981,7 @@
       <c r="S147" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T147" t="n">
-        <v>23.35257110363712</v>
-      </c>
+      <c r="T147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -10835,9 +11051,7 @@
       <c r="S148" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T148" t="n">
-        <v>15.30540194971817</v>
-      </c>
+      <c r="T148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -10977,9 +11191,7 @@
       <c r="S150" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T150" t="n">
-        <v>24.14412989876932</v>
-      </c>
+      <c r="T150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -11049,9 +11261,7 @@
       <c r="S151" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T151" t="n">
-        <v>27.73028609994433</v>
-      </c>
+      <c r="T151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -11401,9 +11611,7 @@
       <c r="S156" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T156" t="n">
-        <v>24.16451719845867</v>
-      </c>
+      <c r="T156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -11473,9 +11681,7 @@
       <c r="S157" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T157" t="n">
-        <v>22.68643009780759</v>
-      </c>
+      <c r="T157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -11545,9 +11751,7 @@
       <c r="S158" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T158" t="n">
-        <v>28.785637379808</v>
-      </c>
+      <c r="T158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -12037,9 +12241,7 @@
       <c r="S165" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T165" t="n">
-        <v>22.89241611234311</v>
-      </c>
+      <c r="T165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -12179,9 +12381,7 @@
       <c r="S167" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T167" t="n">
-        <v>18.58185241261564</v>
-      </c>
+      <c r="T167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -12251,9 +12451,7 @@
       <c r="S168" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T168" t="n">
-        <v>29.31584343996604</v>
-      </c>
+      <c r="T168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -12323,9 +12521,7 @@
       <c r="S169" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T169" t="n">
-        <v>26.18590453513018</v>
-      </c>
+      <c r="T169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -12535,9 +12731,7 @@
       <c r="S172" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T172" t="n">
-        <v>27.79947454185928</v>
-      </c>
+      <c r="T172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -12607,9 +12801,7 @@
       <c r="S173" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T173" t="n">
-        <v>18.63964296111832</v>
-      </c>
+      <c r="T173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -12679,9 +12871,7 @@
       <c r="S174" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T174" t="n">
-        <v>27.05512223460621</v>
-      </c>
+      <c r="T174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -12751,9 +12941,7 @@
       <c r="S175" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T175" t="n">
-        <v>35.93819616904451</v>
-      </c>
+      <c r="T175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -12823,9 +13011,7 @@
       <c r="S176" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T176" t="n">
-        <v>28.68315797216826</v>
-      </c>
+      <c r="T176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -12895,9 +13081,7 @@
       <c r="S177" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T177" t="n">
-        <v>35.32087710659708</v>
-      </c>
+      <c r="T177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -12967,9 +13151,7 @@
       <c r="S178" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T178" t="n">
-        <v>36.05027655013024</v>
-      </c>
+      <c r="T178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -13039,9 +13221,7 @@
       <c r="S179" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T179" t="n">
-        <v>34.10530071768536</v>
-      </c>
+      <c r="T179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -13111,9 +13291,7 @@
       <c r="S180" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T180" t="n">
-        <v>31.72592396882833</v>
-      </c>
+      <c r="T180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -13183,9 +13361,7 @@
       <c r="S181" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T181" t="n">
-        <v>38.53997763132315</v>
-      </c>
+      <c r="T181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -13255,9 +13431,7 @@
       <c r="S182" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T182" t="n">
-        <v>39.05209697061111</v>
-      </c>
+      <c r="T182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -13327,9 +13501,7 @@
       <c r="S183" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T183" t="n">
-        <v>41.81538482065801</v>
-      </c>
+      <c r="T183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -13399,9 +13571,7 @@
       <c r="S184" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T184" t="n">
-        <v>28.02380774576302</v>
-      </c>
+      <c r="T184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -13471,9 +13641,7 @@
       <c r="S185" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T185" t="n">
-        <v>23.61606748622055</v>
-      </c>
+      <c r="T185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -13543,9 +13711,7 @@
       <c r="S186" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T186" t="n">
-        <v>31.97398626399098</v>
-      </c>
+      <c r="T186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -13615,9 +13781,7 @@
       <c r="S187" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T187" t="n">
-        <v>29.03165121712465</v>
-      </c>
+      <c r="T187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -13687,9 +13851,7 @@
       <c r="S188" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T188" t="n">
-        <v>27.25143696399388</v>
-      </c>
+      <c r="T188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -13759,9 +13921,7 @@
       <c r="S189" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T189" t="n">
-        <v>25.20390857356536</v>
-      </c>
+      <c r="T189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -13831,9 +13991,7 @@
       <c r="S190" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T190" t="n">
-        <v>25.1858033686573</v>
-      </c>
+      <c r="T190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -13903,9 +14061,7 @@
       <c r="S191" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T191" t="n">
-        <v>32.79705868977337</v>
-      </c>
+      <c r="T191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -13975,9 +14131,7 @@
       <c r="S192" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T192" t="n">
-        <v>34.10612544738173</v>
-      </c>
+      <c r="T192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -14047,9 +14201,7 @@
       <c r="S193" t="n">
         <v>0.2942581907953586</v>
       </c>
-      <c r="T193" t="n">
-        <v>19.06544537039708</v>
-      </c>
+      <c r="T193" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add diagonal to carapace
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_Filtered_Data_with_real_length.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U193"/>
+  <dimension ref="A1:V193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,10 +531,15 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>Length_fov(mm)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>RealLength(cm)</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Pond_Type</t>
         </is>
@@ -609,9 +614,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T2" t="n">
-        <v>38.4633237865796</v>
-      </c>
-      <c r="U2" t="inlineStr">
+        <v>37.54470511578233</v>
+      </c>
+      <c r="U2" t="n">
+        <v>37.68534393652742</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -686,9 +694,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T3" t="n">
-        <v>28.90841249553062</v>
-      </c>
-      <c r="U3" t="inlineStr">
+        <v>28.21799354970958</v>
+      </c>
+      <c r="U3" t="n">
+        <v>28.32369541431034</v>
+      </c>
+      <c r="V3" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -763,9 +774,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T4" t="n">
-        <v>39.58479455863773</v>
-      </c>
-      <c r="U4" t="inlineStr">
+        <v>38.63939182737593</v>
+      </c>
+      <c r="U4" t="n">
+        <v>38.78413123827693</v>
+      </c>
+      <c r="V4" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -840,9 +854,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T5" t="n">
-        <v>25.08731753405586</v>
-      </c>
-      <c r="U5" t="inlineStr">
+        <v>24.48815771066471</v>
+      </c>
+      <c r="U5" t="n">
+        <v>24.57988797228289</v>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -917,9 +934,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T6" t="n">
-        <v>22.56153606765636</v>
-      </c>
-      <c r="U6" t="inlineStr">
+        <v>22.02269942450471</v>
+      </c>
+      <c r="U6" t="n">
+        <v>22.10519431871509</v>
+      </c>
+      <c r="V6" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -994,9 +1014,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T7" t="n">
-        <v>25.0324391292011</v>
-      </c>
-      <c r="U7" t="inlineStr">
+        <v>24.43458996548156</v>
+      </c>
+      <c r="U7" t="n">
+        <v>24.52611956752632</v>
+      </c>
+      <c r="V7" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1071,9 +1094,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T8" t="n">
-        <v>35.92035186635304</v>
-      </c>
-      <c r="U8" t="inlineStr">
+        <v>35.06246693500572</v>
+      </c>
+      <c r="U8" t="n">
+        <v>35.19380753248667</v>
+      </c>
+      <c r="V8" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1148,9 +1174,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T9" t="n">
-        <v>33.25101619038021</v>
-      </c>
-      <c r="U9" t="inlineStr">
+        <v>32.45688294113347</v>
+      </c>
+      <c r="U9" t="n">
+        <v>32.57846327390812</v>
+      </c>
+      <c r="V9" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1225,9 +1254,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T10" t="n">
-        <v>25.66259612043985</v>
-      </c>
-      <c r="U10" t="inlineStr">
+        <v>25.04969693189933</v>
+      </c>
+      <c r="U10" t="n">
+        <v>25.14353066492934</v>
+      </c>
+      <c r="V10" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1302,9 +1334,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T11" t="n">
-        <v>29.99930527034374</v>
-      </c>
-      <c r="U11" t="inlineStr">
+        <v>29.28283255765788</v>
+      </c>
+      <c r="U11" t="n">
+        <v>29.39252320581413</v>
+      </c>
+      <c r="V11" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1379,9 +1414,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T12" t="n">
-        <v>36.77899511119482</v>
-      </c>
-      <c r="U12" t="inlineStr">
+        <v>35.90060322312576</v>
+      </c>
+      <c r="U12" t="n">
+        <v>36.03508339778069</v>
+      </c>
+      <c r="V12" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1456,9 +1494,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T13" t="n">
-        <v>29.85513969827502</v>
-      </c>
-      <c r="U13" t="inlineStr">
+        <v>29.14211008860656</v>
+      </c>
+      <c r="U13" t="n">
+        <v>29.25127360405425</v>
+      </c>
+      <c r="V13" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1533,9 +1574,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T14" t="n">
-        <v>30.6454209858543</v>
-      </c>
-      <c r="U14" t="inlineStr">
+        <v>29.91351710650545</v>
+      </c>
+      <c r="U14" t="n">
+        <v>30.02557023775854</v>
+      </c>
+      <c r="V14" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1610,9 +1654,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T15" t="n">
-        <v>33.6003689178345</v>
-      </c>
-      <c r="U15" t="inlineStr">
+        <v>32.7978920854925</v>
+      </c>
+      <c r="U15" t="n">
+        <v>32.92074980541876</v>
+      </c>
+      <c r="V15" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1687,9 +1734,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T16" t="n">
-        <v>14.88120358976283</v>
-      </c>
-      <c r="U16" t="inlineStr">
+        <v>14.52579614922694</v>
+      </c>
+      <c r="U16" t="n">
+        <v>14.58020837152329</v>
+      </c>
+      <c r="V16" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1764,9 +1814,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T17" t="n">
-        <v>26.3800861266348</v>
-      </c>
-      <c r="U17" t="inlineStr">
+        <v>25.75005114090062</v>
+      </c>
+      <c r="U17" t="n">
+        <v>25.84650833281128</v>
+      </c>
+      <c r="V17" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1841,9 +1894,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T18" t="n">
-        <v>35.82629067865172</v>
-      </c>
-      <c r="U18" t="inlineStr">
+        <v>34.97065220847087</v>
+      </c>
+      <c r="U18" t="n">
+        <v>35.10164887689906</v>
+      </c>
+      <c r="V18" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1918,9 +1974,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T19" t="n">
-        <v>29.95368238432675</v>
-      </c>
-      <c r="U19" t="inlineStr">
+        <v>29.23829928197056</v>
+      </c>
+      <c r="U19" t="n">
+        <v>29.34782311279911</v>
+      </c>
+      <c r="V19" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -1995,9 +2054,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T20" t="n">
-        <v>40.83064690332304</v>
-      </c>
-      <c r="U20" t="inlineStr">
+        <v>39.85548950937959</v>
+      </c>
+      <c r="U20" t="n">
+        <v>40.00478430414579</v>
+      </c>
+      <c r="V20" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2072,9 +2134,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T21" t="n">
-        <v>31.81792909839421</v>
-      </c>
-      <c r="U21" t="inlineStr">
+        <v>31.05802223496066</v>
+      </c>
+      <c r="U21" t="n">
+        <v>31.17436257132313</v>
+      </c>
+      <c r="V21" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2149,9 +2214,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T22" t="n">
-        <v>39.09854501863349</v>
-      </c>
-      <c r="U22" t="inlineStr">
+        <v>38.16475537386918</v>
+      </c>
+      <c r="U22" t="n">
+        <v>38.30771684269025</v>
+      </c>
+      <c r="V22" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2226,9 +2294,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T23" t="n">
-        <v>32.60443710561533</v>
-      </c>
-      <c r="U23" t="inlineStr">
+        <v>31.82574608966876</v>
+      </c>
+      <c r="U23" t="n">
+        <v>31.94496224506486</v>
+      </c>
+      <c r="V23" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2303,9 +2374,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T24" t="n">
-        <v>33.74812852721058</v>
-      </c>
-      <c r="U24" t="inlineStr">
+        <v>32.94212275554145</v>
+      </c>
+      <c r="U24" t="n">
+        <v>33.06552074955665</v>
+      </c>
+      <c r="V24" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2380,9 +2454,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T25" t="n">
-        <v>13.4375697239241</v>
-      </c>
-      <c r="U25" t="inlineStr">
+        <v>13.11664055755694</v>
+      </c>
+      <c r="U25" t="n">
+        <v>13.16577421979942</v>
+      </c>
+      <c r="V25" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2457,9 +2534,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T26" t="n">
-        <v>40.86265353499343</v>
-      </c>
-      <c r="U26" t="inlineStr">
+        <v>39.88673172740741</v>
+      </c>
+      <c r="U26" t="n">
+        <v>40.03614355248952</v>
+      </c>
+      <c r="V26" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2534,9 +2614,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T27" t="n">
-        <v>26.71088638279051</v>
-      </c>
-      <c r="U27" t="inlineStr">
+        <v>26.07295090220322</v>
+      </c>
+      <c r="U27" t="n">
+        <v>26.17061764527452</v>
+      </c>
+      <c r="V27" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -2611,7 +2694,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr">
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2686,7 +2770,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2761,7 +2846,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2836,7 +2922,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2911,7 +2998,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr">
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2986,7 +3074,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr">
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3061,7 +3150,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3136,9 +3226,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T35" t="n">
-        <v>29.66716495857016</v>
-      </c>
-      <c r="U35" t="inlineStr">
+        <v>28.95862474525468</v>
+      </c>
+      <c r="U35" t="n">
+        <v>29.06710094241785</v>
+      </c>
+      <c r="V35" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3213,9 +3306,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T36" t="n">
-        <v>38.57159027353561</v>
-      </c>
-      <c r="U36" t="inlineStr">
+        <v>37.65038587673889</v>
+      </c>
+      <c r="U36" t="n">
+        <v>37.79142056735568</v>
+      </c>
+      <c r="V36" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3290,9 +3386,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T37" t="n">
-        <v>25.38946462654251</v>
-      </c>
-      <c r="U37" t="inlineStr">
+        <v>24.78308863114227</v>
+      </c>
+      <c r="U37" t="n">
+        <v>24.8759236753584</v>
+      </c>
+      <c r="V37" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3367,9 +3466,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T38" t="n">
-        <v>41.82014928176122</v>
-      </c>
-      <c r="U38" t="inlineStr">
+        <v>40.82135962544037</v>
+      </c>
+      <c r="U38" t="n">
+        <v>40.97427247590035</v>
+      </c>
+      <c r="V38" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3444,9 +3546,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T39" t="n">
-        <v>40.6362236076846</v>
-      </c>
-      <c r="U39" t="inlineStr">
+        <v>39.66570962080609</v>
+      </c>
+      <c r="U39" t="n">
+        <v>39.8142935185324</v>
+      </c>
+      <c r="V39" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3521,9 +3626,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T40" t="n">
-        <v>24.59366620671134</v>
-      </c>
-      <c r="U40" t="inlineStr">
+        <v>24.00629624653322</v>
+      </c>
+      <c r="U40" t="n">
+        <v>24.09622150188304</v>
+      </c>
+      <c r="V40" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3598,9 +3706,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T41" t="n">
-        <v>38.88348622483628</v>
-      </c>
-      <c r="U41" t="inlineStr">
+        <v>37.95483282426131</v>
+      </c>
+      <c r="U41" t="n">
+        <v>38.0970079435896</v>
+      </c>
+      <c r="V41" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3677,7 +3788,10 @@
       <c r="T42" t="n">
         <v>0</v>
       </c>
-      <c r="U42" t="inlineStr">
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3752,9 +3866,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T43" t="n">
-        <v>37.25549928137975</v>
-      </c>
-      <c r="U43" t="inlineStr">
+        <v>36.36572705525479</v>
+      </c>
+      <c r="U43" t="n">
+        <v>36.5019495386334</v>
+      </c>
+      <c r="V43" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3829,9 +3946,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T44" t="n">
-        <v>28.29811256526354</v>
-      </c>
-      <c r="U44" t="inlineStr">
+        <v>27.62226939853638</v>
+      </c>
+      <c r="U44" t="n">
+        <v>27.72573973829624</v>
+      </c>
+      <c r="V44" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3906,9 +4026,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T45" t="n">
-        <v>31.1195526044811</v>
-      </c>
-      <c r="U45" t="inlineStr">
+        <v>30.37632505067024</v>
+      </c>
+      <c r="U45" t="n">
+        <v>30.49011181555551</v>
+      </c>
+      <c r="V45" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -3983,9 +4106,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T46" t="n">
-        <v>31.1195526044811</v>
-      </c>
-      <c r="U46" t="inlineStr">
+        <v>30.37632505067024</v>
+      </c>
+      <c r="U46" t="n">
+        <v>30.49011181555551</v>
+      </c>
+      <c r="V46" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4060,9 +4186,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T47" t="n">
-        <v>27.31090890939526</v>
-      </c>
-      <c r="U47" t="inlineStr">
+        <v>26.65864310470764</v>
+      </c>
+      <c r="U47" t="n">
+        <v>26.75850379391397</v>
+      </c>
+      <c r="V47" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4137,9 +4266,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T48" t="n">
-        <v>35.69938430494975</v>
-      </c>
-      <c r="U48" t="inlineStr">
+        <v>34.84677673675159</v>
+      </c>
+      <c r="U48" t="n">
+        <v>34.97730937968782</v>
+      </c>
+      <c r="V48" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4214,9 +4346,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T49" t="n">
-        <v>35.66872639569743</v>
-      </c>
-      <c r="U49" t="inlineStr">
+        <v>34.81685102963561</v>
+      </c>
+      <c r="U49" t="n">
+        <v>34.94727157377799</v>
+      </c>
+      <c r="V49" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4291,9 +4426,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T50" t="n">
-        <v>37.80206187604055</v>
-      </c>
-      <c r="U50" t="inlineStr">
+        <v>36.89923610813118</v>
+      </c>
+      <c r="U50" t="n">
+        <v>37.03745706463196</v>
+      </c>
+      <c r="V50" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4368,9 +4506,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T51" t="n">
-        <v>27.27328331517984</v>
-      </c>
-      <c r="U51" t="inlineStr">
+        <v>26.62191612168707</v>
+      </c>
+      <c r="U51" t="n">
+        <v>26.72163923518025</v>
+      </c>
+      <c r="V51" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4445,9 +4586,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T52" t="n">
-        <v>32.61034635295254</v>
-      </c>
-      <c r="U52" t="inlineStr">
+        <v>31.83151420658873</v>
+      </c>
+      <c r="U52" t="n">
+        <v>31.95075196879088</v>
+      </c>
+      <c r="V52" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4522,9 +4666,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T53" t="n">
-        <v>33.05552903157839</v>
-      </c>
-      <c r="U53" t="inlineStr">
+        <v>32.26606459761587</v>
+      </c>
+      <c r="U53" t="n">
+        <v>32.38693014339922</v>
+      </c>
+      <c r="V53" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4599,9 +4746,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T54" t="n">
-        <v>32.94869791238239</v>
-      </c>
-      <c r="U54" t="inlineStr">
+        <v>32.16178492356434</v>
+      </c>
+      <c r="U54" t="n">
+        <v>32.28225984781155</v>
+      </c>
+      <c r="V54" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4676,9 +4826,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T55" t="n">
-        <v>37.9223596053432</v>
-      </c>
-      <c r="U55" t="inlineStr">
+        <v>37.01666076955221</v>
+      </c>
+      <c r="U55" t="n">
+        <v>37.15532158743577</v>
+      </c>
+      <c r="V55" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4753,9 +4906,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T56" t="n">
-        <v>22.77184097144083</v>
-      </c>
-      <c r="U56" t="inlineStr">
+        <v>22.22798162114488</v>
+      </c>
+      <c r="U56" t="n">
+        <v>22.31124548253629</v>
+      </c>
+      <c r="V56" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4830,9 +4986,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T57" t="n">
-        <v>29.37688020749116</v>
-      </c>
-      <c r="U57" t="inlineStr">
+        <v>28.67527285815979</v>
+      </c>
+      <c r="U57" t="n">
+        <v>28.78268764666003</v>
+      </c>
+      <c r="V57" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4907,9 +5066,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T58" t="n">
-        <v>41.04519345454099</v>
-      </c>
-      <c r="U58" t="inlineStr">
+        <v>40.06491205028588</v>
+      </c>
+      <c r="U58" t="n">
+        <v>40.2149913215608</v>
+      </c>
+      <c r="V58" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -4984,9 +5146,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T59" t="n">
-        <v>41.04519345454099</v>
-      </c>
-      <c r="U59" t="inlineStr">
+        <v>40.06491205028588</v>
+      </c>
+      <c r="U59" t="n">
+        <v>40.2149913215608</v>
+      </c>
+      <c r="V59" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5061,9 +5226,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T60" t="n">
-        <v>22.77184097144083</v>
-      </c>
-      <c r="U60" t="inlineStr">
+        <v>22.22798162114488</v>
+      </c>
+      <c r="U60" t="n">
+        <v>22.31124548253629</v>
+      </c>
+      <c r="V60" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5138,9 +5306,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T61" t="n">
-        <v>5.932218397323056</v>
-      </c>
-      <c r="U61" t="inlineStr">
+        <v>5.790539362789659</v>
+      </c>
+      <c r="U61" t="n">
+        <v>5.812230161131247</v>
+      </c>
+      <c r="V61" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5215,9 +5386,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T62" t="n">
-        <v>36.2494911237218</v>
-      </c>
-      <c r="U62" t="inlineStr">
+        <v>35.38374536711692</v>
+      </c>
+      <c r="U62" t="n">
+        <v>35.51628944241674</v>
+      </c>
+      <c r="V62" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5292,9 +5466,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T63" t="n">
-        <v>22.68334623615863</v>
-      </c>
-      <c r="U63" t="inlineStr">
+        <v>22.141600403575</v>
+      </c>
+      <c r="U63" t="n">
+        <v>22.22454068931076</v>
+      </c>
+      <c r="V63" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5369,9 +5546,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T64" t="n">
-        <v>21.4270352236767</v>
-      </c>
-      <c r="U64" t="inlineStr">
+        <v>20.91529383789537</v>
+      </c>
+      <c r="U64" t="n">
+        <v>20.99364049827871</v>
+      </c>
+      <c r="V64" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5446,9 +5626,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T65" t="n">
-        <v>44.6018161614268</v>
-      </c>
-      <c r="U65" t="inlineStr">
+        <v>43.53659201947029</v>
+      </c>
+      <c r="U65" t="n">
+        <v>43.69967586689955</v>
+      </c>
+      <c r="V65" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5523,9 +5706,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T66" t="n">
-        <v>32.86013969936226</v>
-      </c>
-      <c r="U66" t="inlineStr">
+        <v>32.07534174429387</v>
+      </c>
+      <c r="U66" t="n">
+        <v>32.19549286078293</v>
+      </c>
+      <c r="V66" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5600,9 +5786,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T67" t="n">
-        <v>23.94292818163721</v>
-      </c>
-      <c r="U67" t="inlineStr">
+        <v>23.3710997826343</v>
+      </c>
+      <c r="U67" t="n">
+        <v>23.45864565369147</v>
+      </c>
+      <c r="V67" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5677,9 +5866,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T68" t="n">
-        <v>32.07007888525862</v>
-      </c>
-      <c r="U68" t="inlineStr">
+        <v>31.3041499343077</v>
+      </c>
+      <c r="U68" t="n">
+        <v>31.42141224113931</v>
+      </c>
+      <c r="V68" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5754,9 +5946,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T69" t="n">
-        <v>40.77401073165723</v>
-      </c>
-      <c r="U69" t="inlineStr">
+        <v>39.80020597808942</v>
+      </c>
+      <c r="U69" t="n">
+        <v>39.949293686114</v>
+      </c>
+      <c r="V69" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5831,9 +6026,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T70" t="n">
-        <v>22.54608821295353</v>
-      </c>
-      <c r="U70" t="inlineStr">
+        <v>22.00762051055782</v>
+      </c>
+      <c r="U70" t="n">
+        <v>22.09005892062033</v>
+      </c>
+      <c r="V70" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5908,9 +6106,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T71" t="n">
-        <v>30.66559632295112</v>
-      </c>
-      <c r="U71" t="inlineStr">
+        <v>29.93321059649385</v>
+      </c>
+      <c r="U71" t="n">
+        <v>30.04533749764872</v>
+      </c>
+      <c r="V71" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -5985,9 +6186,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T72" t="n">
-        <v>36.78868115922425</v>
-      </c>
-      <c r="U72" t="inlineStr">
+        <v>35.91005793949454</v>
+      </c>
+      <c r="U72" t="n">
+        <v>36.04457353059917</v>
+      </c>
+      <c r="V72" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6062,9 +6266,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T73" t="n">
-        <v>35.61726580577677</v>
-      </c>
-      <c r="U73" t="inlineStr">
+        <v>34.76661947179167</v>
+      </c>
+      <c r="U73" t="n">
+        <v>34.89685185339456</v>
+      </c>
+      <c r="V73" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6139,9 +6346,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T74" t="n">
-        <v>35.98502691473605</v>
-      </c>
-      <c r="U74" t="inlineStr">
+        <v>35.12559735070672</v>
+      </c>
+      <c r="U74" t="n">
+        <v>35.25717442859657</v>
+      </c>
+      <c r="V74" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6216,9 +6426,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T75" t="n">
-        <v>37.28961843891066</v>
-      </c>
-      <c r="U75" t="inlineStr">
+        <v>36.39903134573694</v>
+      </c>
+      <c r="U75" t="n">
+        <v>36.5353785837547</v>
+      </c>
+      <c r="V75" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6293,9 +6506,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T76" t="n">
-        <v>37.15197798132769</v>
-      </c>
-      <c r="U76" t="inlineStr">
+        <v>36.26467815201328</v>
+      </c>
+      <c r="U76" t="n">
+        <v>36.40052211600958</v>
+      </c>
+      <c r="V76" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6370,9 +6586,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T77" t="n">
-        <v>27.89060114459023</v>
-      </c>
-      <c r="U77" t="inlineStr">
+        <v>27.22449056368094</v>
+      </c>
+      <c r="U77" t="n">
+        <v>27.32647086253946</v>
+      </c>
+      <c r="V77" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6447,9 +6666,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T78" t="n">
-        <v>26.24450967504827</v>
-      </c>
-      <c r="U78" t="inlineStr">
+        <v>25.61771265856601</v>
+      </c>
+      <c r="U78" t="n">
+        <v>25.7136741233685</v>
+      </c>
+      <c r="V78" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6524,9 +6746,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T79" t="n">
-        <v>32.27511536018605</v>
-      </c>
-      <c r="U79" t="inlineStr">
+        <v>31.50428952785515</v>
+      </c>
+      <c r="U79" t="n">
+        <v>31.62230153817581</v>
+      </c>
+      <c r="V79" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6601,9 +6826,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T80" t="n">
-        <v>33.05232270520634</v>
-      </c>
-      <c r="U80" t="inlineStr">
+        <v>32.26293484786228</v>
+      </c>
+      <c r="U80" t="n">
+        <v>32.38378866990686</v>
+      </c>
+      <c r="V80" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6678,9 +6906,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T81" t="n">
-        <v>37.91380773744524</v>
-      </c>
-      <c r="U81" t="inlineStr">
+        <v>37.00831314571712</v>
+      </c>
+      <c r="U81" t="n">
+        <v>37.14694269421212</v>
+      </c>
+      <c r="V81" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6755,9 +6986,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T82" t="n">
-        <v>21.69298224001026</v>
-      </c>
-      <c r="U82" t="inlineStr">
+        <v>21.17488924779984</v>
+      </c>
+      <c r="U82" t="n">
+        <v>21.2542083273887</v>
+      </c>
+      <c r="V82" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6832,9 +7066,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T83" t="n">
-        <v>38.9287987021165</v>
-      </c>
-      <c r="U83" t="inlineStr">
+        <v>37.99906310469654</v>
+      </c>
+      <c r="U83" t="n">
+        <v>38.14140390636172</v>
+      </c>
+      <c r="V83" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6909,9 +7146,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T84" t="n">
-        <v>29.76221372731837</v>
-      </c>
-      <c r="U84" t="inlineStr">
+        <v>29.05140346646117</v>
+      </c>
+      <c r="U84" t="n">
+        <v>29.16022720370756</v>
+      </c>
+      <c r="V84" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -6986,9 +7226,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T85" t="n">
-        <v>41.09995843088404</v>
-      </c>
-      <c r="U85" t="inlineStr">
+        <v>40.11836907596783</v>
+      </c>
+      <c r="U85" t="n">
+        <v>40.26864859207166</v>
+      </c>
+      <c r="V85" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7063,9 +7306,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T86" t="n">
-        <v>33.02120064349632</v>
-      </c>
-      <c r="U86" t="inlineStr">
+        <v>32.23255607363096</v>
+      </c>
+      <c r="U86" t="n">
+        <v>32.35329609973628</v>
+      </c>
+      <c r="V86" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7140,9 +7386,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T87" t="n">
-        <v>29.65910939016912</v>
-      </c>
-      <c r="U87" t="inlineStr">
+        <v>28.95076156780713</v>
+      </c>
+      <c r="U87" t="n">
+        <v>29.05920831027088</v>
+      </c>
+      <c r="V87" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7217,9 +7466,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T88" t="n">
-        <v>30.11506256205754</v>
-      </c>
-      <c r="U88" t="inlineStr">
+        <v>29.39582522065579</v>
+      </c>
+      <c r="U88" t="n">
+        <v>29.50593912835896</v>
+      </c>
+      <c r="V88" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7294,9 +7546,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T89" t="n">
-        <v>37.16291925265281</v>
-      </c>
-      <c r="U89" t="inlineStr">
+        <v>36.27535811320885</v>
+      </c>
+      <c r="U89" t="n">
+        <v>36.41124208330304</v>
+      </c>
+      <c r="V89" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7371,9 +7626,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T90" t="n">
-        <v>39.37405917893729</v>
-      </c>
-      <c r="U90" t="inlineStr">
+        <v>38.43368943586612</v>
+      </c>
+      <c r="U90" t="n">
+        <v>38.5776583055769</v>
+      </c>
+      <c r="V90" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7448,9 +7706,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T91" t="n">
-        <v>28.15365666098232</v>
-      </c>
-      <c r="U91" t="inlineStr">
+        <v>27.48126353127006</v>
+      </c>
+      <c r="U91" t="n">
+        <v>27.58420567673915</v>
+      </c>
+      <c r="V91" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7525,9 +7786,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T92" t="n">
-        <v>36.02324033101383</v>
-      </c>
-      <c r="U92" t="inlineStr">
+        <v>35.16289811684894</v>
+      </c>
+      <c r="U92" t="n">
+        <v>35.29461491978782</v>
+      </c>
+      <c r="V92" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7602,9 +7866,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T93" t="n">
-        <v>36.02324033101383</v>
-      </c>
-      <c r="U93" t="inlineStr">
+        <v>35.16289811684894</v>
+      </c>
+      <c r="U93" t="n">
+        <v>35.29461491978782</v>
+      </c>
+      <c r="V93" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7679,9 +7946,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T94" t="n">
-        <v>42.04655497189034</v>
-      </c>
-      <c r="U94" t="inlineStr">
+        <v>41.04235807371798</v>
+      </c>
+      <c r="U94" t="n">
+        <v>41.19609876291198</v>
+      </c>
+      <c r="V94" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7756,9 +8026,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T95" t="n">
-        <v>42.04655497189034</v>
-      </c>
-      <c r="U95" t="inlineStr">
+        <v>41.04235807371798</v>
+      </c>
+      <c r="U95" t="n">
+        <v>41.19609876291198</v>
+      </c>
+      <c r="V95" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7833,9 +8106,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T96" t="n">
-        <v>28.55569977185347</v>
-      </c>
-      <c r="U96" t="inlineStr">
+        <v>27.87370465583963</v>
+      </c>
+      <c r="U96" t="n">
+        <v>27.9781168476655</v>
+      </c>
+      <c r="V96" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7910,9 +8186,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T97" t="n">
-        <v>25.08352199801356</v>
-      </c>
-      <c r="U97" t="inlineStr">
+        <v>24.48445282332177</v>
+      </c>
+      <c r="U97" t="n">
+        <v>24.5761692067916</v>
+      </c>
+      <c r="V97" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -7987,9 +8266,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T98" t="n">
-        <v>32.10890210100942</v>
-      </c>
-      <c r="U98" t="inlineStr">
+        <v>31.34204593609627</v>
+      </c>
+      <c r="U98" t="n">
+        <v>31.45945019767185</v>
+      </c>
+      <c r="V98" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -8064,9 +8346,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T99" t="n">
-        <v>35.24787868406799</v>
-      </c>
-      <c r="U99" t="inlineStr">
+        <v>34.40605441415193</v>
+      </c>
+      <c r="U99" t="n">
+        <v>34.53493615405043</v>
+      </c>
+      <c r="V99" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -8141,9 +8426,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T100" t="n">
-        <v>26.40099503999025</v>
-      </c>
-      <c r="U100" t="inlineStr">
+        <v>25.77046068716286</v>
+      </c>
+      <c r="U100" t="n">
+        <v>25.86699433125258</v>
+      </c>
+      <c r="V100" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8218,9 +8506,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T101" t="n">
-        <v>24.30590653746043</v>
-      </c>
-      <c r="U101" t="inlineStr">
+        <v>23.72540913479563</v>
+      </c>
+      <c r="U101" t="n">
+        <v>23.81428221429173</v>
+      </c>
+      <c r="V101" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8295,9 +8586,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T102" t="n">
-        <v>28.70858223280479</v>
-      </c>
-      <c r="U102" t="inlineStr">
+        <v>28.02293582851836</v>
+      </c>
+      <c r="U102" t="n">
+        <v>28.12790702583059</v>
+      </c>
+      <c r="V102" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8372,9 +8666,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T103" t="n">
-        <v>16.66960532839994</v>
-      </c>
-      <c r="U103" t="inlineStr">
+        <v>16.27148553057756</v>
+      </c>
+      <c r="U103" t="n">
+        <v>16.33243693583522</v>
+      </c>
+      <c r="V103" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8449,9 +8746,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T104" t="n">
-        <v>41.69927347902058</v>
-      </c>
-      <c r="U104" t="inlineStr">
+        <v>40.70337069669589</v>
+      </c>
+      <c r="U104" t="n">
+        <v>40.85584157208247</v>
+      </c>
+      <c r="V104" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -8526,9 +8826,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T105" t="n">
-        <v>33.65194007901309</v>
-      </c>
-      <c r="U105" t="inlineStr">
+        <v>32.84823157382357</v>
+      </c>
+      <c r="U105" t="n">
+        <v>32.97127786058645</v>
+      </c>
+      <c r="V105" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -8603,9 +8906,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T106" t="n">
-        <v>19.81466091885927</v>
-      </c>
-      <c r="U106" t="inlineStr">
+        <v>19.34142783124108</v>
+      </c>
+      <c r="U106" t="n">
+        <v>19.41387894234513</v>
+      </c>
+      <c r="V106" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8680,9 +8986,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T107" t="n">
-        <v>27.76297519301385</v>
-      </c>
-      <c r="U107" t="inlineStr">
+        <v>27.09991269974896</v>
+      </c>
+      <c r="U107" t="n">
+        <v>27.20142634202247</v>
+      </c>
+      <c r="V107" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8757,9 +9066,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T108" t="n">
-        <v>24.99403917041211</v>
-      </c>
-      <c r="U108" t="inlineStr">
+        <v>24.39710711201861</v>
+      </c>
+      <c r="U108" t="n">
+        <v>24.48849630693291</v>
+      </c>
+      <c r="V108" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8834,9 +9146,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T109" t="n">
-        <v>11.77376306918397</v>
-      </c>
-      <c r="U109" t="inlineStr">
+        <v>11.49257055860147</v>
+      </c>
+      <c r="U109" t="n">
+        <v>11.535620612283</v>
+      </c>
+      <c r="V109" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -8911,9 +9226,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T110" t="n">
-        <v>27.55312813747785</v>
-      </c>
-      <c r="U110" t="inlineStr">
+        <v>26.89507741657816</v>
+      </c>
+      <c r="U110" t="n">
+        <v>26.9958237657651</v>
+      </c>
+      <c r="V110" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -8988,9 +9306,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T111" t="n">
-        <v>30.50735045245302</v>
-      </c>
-      <c r="U111" t="inlineStr">
+        <v>29.7787441084543</v>
+      </c>
+      <c r="U111" t="n">
+        <v>29.89029239313965</v>
+      </c>
+      <c r="V111" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9065,9 +9386,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T112" t="n">
-        <v>30.35488466805121</v>
-      </c>
-      <c r="U112" t="inlineStr">
+        <v>29.62991966084871</v>
+      </c>
+      <c r="U112" t="n">
+        <v>29.74091046360033</v>
+      </c>
+      <c r="V112" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9142,9 +9466,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T113" t="n">
-        <v>36.95209972476533</v>
-      </c>
-      <c r="U113" t="inlineStr">
+        <v>36.0695735832212</v>
+      </c>
+      <c r="U113" t="n">
+        <v>36.2046867044424</v>
+      </c>
+      <c r="V113" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9219,9 +9546,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T114" t="n">
-        <v>38.28643206145068</v>
-      </c>
-      <c r="U114" t="inlineStr">
+        <v>37.37203809162606</v>
+      </c>
+      <c r="U114" t="n">
+        <v>37.51203011846017</v>
+      </c>
+      <c r="V114" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9296,9 +9626,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T115" t="n">
-        <v>31.30521510351421</v>
-      </c>
-      <c r="U115" t="inlineStr">
+        <v>30.55755337654076</v>
+      </c>
+      <c r="U115" t="n">
+        <v>30.67201900514216</v>
+      </c>
+      <c r="V115" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9373,9 +9706,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T116" t="n">
-        <v>31.30521510351421</v>
-      </c>
-      <c r="U116" t="inlineStr">
+        <v>30.55755337654076</v>
+      </c>
+      <c r="U116" t="n">
+        <v>30.67201900514216</v>
+      </c>
+      <c r="V116" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9450,9 +9786,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T117" t="n">
-        <v>39.32170888326723</v>
-      </c>
-      <c r="U117" t="inlineStr">
+        <v>38.38258942109459</v>
+      </c>
+      <c r="U117" t="n">
+        <v>38.52636687511053</v>
+      </c>
+      <c r="V117" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9527,9 +9866,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T118" t="n">
-        <v>25.9641771671566</v>
-      </c>
-      <c r="U118" t="inlineStr">
+        <v>25.344075325465</v>
+      </c>
+      <c r="U118" t="n">
+        <v>25.43901177138077</v>
+      </c>
+      <c r="V118" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9604,9 +9946,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T119" t="n">
-        <v>47.34216650991087</v>
-      </c>
-      <c r="U119" t="inlineStr">
+        <v>46.21149464407561</v>
+      </c>
+      <c r="U119" t="n">
+        <v>46.38459841707287</v>
+      </c>
+      <c r="V119" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9681,9 +10026,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T120" t="n">
-        <v>27.33787097916291</v>
-      </c>
-      <c r="U120" t="inlineStr">
+        <v>26.68496123998773</v>
+      </c>
+      <c r="U120" t="n">
+        <v>26.78492051437401</v>
+      </c>
+      <c r="V120" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9758,9 +10106,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T121" t="n">
-        <v>30.76737122817728</v>
-      </c>
-      <c r="U121" t="inlineStr">
+        <v>30.03255481401662</v>
+      </c>
+      <c r="U121" t="n">
+        <v>30.14505384896658</v>
+      </c>
+      <c r="V121" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9835,9 +10186,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T122" t="n">
-        <v>35.66874734664732</v>
-      </c>
-      <c r="U122" t="inlineStr">
+        <v>34.81687148021443</v>
+      </c>
+      <c r="U122" t="n">
+        <v>34.94729210096271</v>
+      </c>
+      <c r="V122" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9912,9 +10266,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T123" t="n">
-        <v>17.70668971733859</v>
-      </c>
-      <c r="U123" t="inlineStr">
+        <v>17.28380125708449</v>
+      </c>
+      <c r="U123" t="n">
+        <v>17.348544698784</v>
+      </c>
+      <c r="V123" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -9989,9 +10346,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T124" t="n">
-        <v>33.17591760582172</v>
-      </c>
-      <c r="U124" t="inlineStr">
+        <v>32.38357793432995</v>
+      </c>
+      <c r="U124" t="n">
+        <v>32.50488367366513</v>
+      </c>
+      <c r="V124" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10066,9 +10426,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T125" t="n">
-        <v>43.44318443566831</v>
-      </c>
-      <c r="U125" t="inlineStr">
+        <v>42.40563186837252</v>
+      </c>
+      <c r="U125" t="n">
+        <v>42.56447924886272</v>
+      </c>
+      <c r="V125" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10143,9 +10506,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T126" t="n">
-        <v>30.54452112120853</v>
-      </c>
-      <c r="U126" t="inlineStr">
+        <v>29.81502703098916</v>
+      </c>
+      <c r="U126" t="n">
+        <v>29.9267112279802</v>
+      </c>
+      <c r="V126" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10220,9 +10586,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T127" t="n">
-        <v>34.7428440738251</v>
-      </c>
-      <c r="U127" t="inlineStr">
+        <v>33.9130815338038</v>
+      </c>
+      <c r="U127" t="n">
+        <v>34.04011664514741</v>
+      </c>
+      <c r="V127" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10297,9 +10666,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T128" t="n">
-        <v>33.38487950600774</v>
-      </c>
-      <c r="U128" t="inlineStr">
+        <v>32.58754920229548</v>
+      </c>
+      <c r="U128" t="n">
+        <v>32.70961899820013</v>
+      </c>
+      <c r="V128" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10374,9 +10746,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T129" t="n">
-        <v>31.42351786084434</v>
-      </c>
-      <c r="U129" t="inlineStr">
+        <v>30.67303071185865</v>
+      </c>
+      <c r="U129" t="n">
+        <v>30.7879289073483</v>
+      </c>
+      <c r="V129" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10451,9 +10826,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T130" t="n">
-        <v>44.99084352523037</v>
-      </c>
-      <c r="U130" t="inlineStr">
+        <v>43.91632825175793</v>
+      </c>
+      <c r="U130" t="n">
+        <v>44.08083455425079</v>
+      </c>
+      <c r="V130" t="inlineStr">
         <is>
           <t>1\carapace\right</t>
         </is>
@@ -10528,9 +10906,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T131" t="n">
-        <v>30.8850707256197</v>
-      </c>
-      <c r="U131" t="inlineStr">
+        <v>30.14744329708874</v>
+      </c>
+      <c r="U131" t="n">
+        <v>30.26037269314357</v>
+      </c>
+      <c r="V131" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10605,9 +10986,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T132" t="n">
-        <v>30.8850707256197</v>
-      </c>
-      <c r="U132" t="inlineStr">
+        <v>30.14744329708874</v>
+      </c>
+      <c r="U132" t="n">
+        <v>30.26037269314357</v>
+      </c>
+      <c r="V132" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10682,9 +11066,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T133" t="n">
-        <v>23.40085017798146</v>
-      </c>
-      <c r="U133" t="inlineStr">
+        <v>22.84196821537988</v>
+      </c>
+      <c r="U133" t="n">
+        <v>22.92753201095109</v>
+      </c>
+      <c r="V133" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10759,9 +11146,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T134" t="n">
-        <v>26.13822724578434</v>
-      </c>
-      <c r="U134" t="inlineStr">
+        <v>25.51396857009762</v>
+      </c>
+      <c r="U134" t="n">
+        <v>25.60954141961557</v>
+      </c>
+      <c r="V134" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10836,9 +11226,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T135" t="n">
-        <v>37.24854587790906</v>
-      </c>
-      <c r="U135" t="inlineStr">
+        <v>36.35893971975808</v>
+      </c>
+      <c r="U135" t="n">
+        <v>36.49513677843679</v>
+      </c>
+      <c r="V135" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10913,9 +11306,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T136" t="n">
-        <v>22.2617911969999</v>
-      </c>
-      <c r="U136" t="inlineStr">
+        <v>21.73011335364903</v>
+      </c>
+      <c r="U136" t="n">
+        <v>21.81151224884051</v>
+      </c>
+      <c r="V136" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -10990,9 +11386,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T137" t="n">
-        <v>36.05057799982835</v>
-      </c>
-      <c r="U137" t="inlineStr">
+        <v>35.18958288075258</v>
+      </c>
+      <c r="U137" t="n">
+        <v>35.32139964222664</v>
+      </c>
+      <c r="V137" t="inlineStr">
         <is>
           <t>1\carapace\left</t>
         </is>
@@ -11067,9 +11466,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T138" t="n">
-        <v>30.27586619575271</v>
-      </c>
-      <c r="U138" t="inlineStr">
+        <v>29.55278838489326</v>
+      </c>
+      <c r="U138" t="n">
+        <v>29.6634902613726</v>
+      </c>
+      <c r="V138" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11144,9 +11546,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T139" t="n">
-        <v>23.8040416050937</v>
-      </c>
-      <c r="U139" t="inlineStr">
+        <v>23.23553023098038</v>
+      </c>
+      <c r="U139" t="n">
+        <v>23.32256827165734</v>
+      </c>
+      <c r="V139" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11221,7 +11626,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T140" t="inlineStr"/>
-      <c r="U140" t="inlineStr">
+      <c r="U140" t="inlineStr"/>
+      <c r="V140" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -11296,9 +11702,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T141" t="n">
-        <v>27.39537848272629</v>
-      </c>
-      <c r="U141" t="inlineStr">
+        <v>26.74109529317596</v>
+      </c>
+      <c r="U141" t="n">
+        <v>26.84126484027632</v>
+      </c>
+      <c r="V141" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11373,9 +11782,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T142" t="n">
-        <v>19.41279162135829</v>
-      </c>
-      <c r="U142" t="inlineStr">
+        <v>18.94915636886098</v>
+      </c>
+      <c r="U142" t="n">
+        <v>19.02013806914635</v>
+      </c>
+      <c r="V142" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11450,7 +11862,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T143" t="inlineStr"/>
-      <c r="U143" t="inlineStr">
+      <c r="U143" t="inlineStr"/>
+      <c r="V143" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -11525,9 +11938,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T144" t="n">
-        <v>21.98143793600146</v>
-      </c>
-      <c r="U144" t="inlineStr">
+        <v>21.45645576308721</v>
+      </c>
+      <c r="U144" t="n">
+        <v>21.53682956350952</v>
+      </c>
+      <c r="V144" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11602,7 +12018,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T145" t="inlineStr"/>
-      <c r="U145" t="inlineStr">
+      <c r="U145" t="inlineStr"/>
+      <c r="V145" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -11677,7 +12094,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T146" t="inlineStr"/>
-      <c r="U146" t="inlineStr">
+      <c r="U146" t="inlineStr"/>
+      <c r="V146" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -11752,9 +12170,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T147" t="n">
-        <v>23.14597641820976</v>
-      </c>
-      <c r="U147" t="inlineStr">
+        <v>22.59318159970737</v>
+      </c>
+      <c r="U147" t="n">
+        <v>22.677813464767</v>
+      </c>
+      <c r="V147" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11829,9 +12250,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T148" t="n">
-        <v>17.79713683116967</v>
-      </c>
-      <c r="U148" t="inlineStr">
+        <v>17.37208822459161</v>
+      </c>
+      <c r="U148" t="n">
+        <v>17.43716238070103</v>
+      </c>
+      <c r="V148" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -11906,7 +12330,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T149" t="inlineStr"/>
-      <c r="U149" t="inlineStr">
+      <c r="U149" t="inlineStr"/>
+      <c r="V149" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -11981,9 +12406,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T150" t="n">
-        <v>25.04892547497485</v>
-      </c>
-      <c r="U150" t="inlineStr">
+        <v>24.45068256824119</v>
+      </c>
+      <c r="U150" t="n">
+        <v>24.54227245161371</v>
+      </c>
+      <c r="V150" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -12058,9 +12486,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T151" t="n">
-        <v>27.05850836230622</v>
-      </c>
-      <c r="U151" t="inlineStr">
+        <v>26.41227063403658</v>
+      </c>
+      <c r="U151" t="n">
+        <v>26.51120843588416</v>
+      </c>
+      <c r="V151" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -12135,7 +12566,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T152" t="inlineStr"/>
-      <c r="U152" t="inlineStr">
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12210,7 +12642,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T153" t="inlineStr"/>
-      <c r="U153" t="inlineStr">
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12285,7 +12718,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T154" t="inlineStr"/>
-      <c r="U154" t="inlineStr">
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12360,7 +12794,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T155" t="inlineStr"/>
-      <c r="U155" t="inlineStr">
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12435,9 +12870,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T156" t="n">
-        <v>23.12833107893655</v>
-      </c>
-      <c r="U156" t="inlineStr">
+        <v>22.57595768366318</v>
+      </c>
+      <c r="U156" t="n">
+        <v>22.66052502960531</v>
+      </c>
+      <c r="V156" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -12512,7 +12950,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T157" t="inlineStr"/>
-      <c r="U157" t="inlineStr">
+      <c r="U157" t="inlineStr"/>
+      <c r="V157" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12587,9 +13026,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T158" t="n">
-        <v>27.78774076759526</v>
-      </c>
-      <c r="U158" t="inlineStr">
+        <v>27.12408679868646</v>
+      </c>
+      <c r="U158" t="n">
+        <v>27.22569099478791</v>
+      </c>
+      <c r="V158" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -12664,7 +13106,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T159" t="inlineStr"/>
-      <c r="U159" t="inlineStr">
+      <c r="U159" t="inlineStr"/>
+      <c r="V159" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12739,7 +13182,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T160" t="inlineStr"/>
-      <c r="U160" t="inlineStr">
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12814,7 +13258,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T161" t="inlineStr"/>
-      <c r="U161" t="inlineStr">
+      <c r="U161" t="inlineStr"/>
+      <c r="V161" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12889,7 +13334,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T162" t="inlineStr"/>
-      <c r="U162" t="inlineStr">
+      <c r="U162" t="inlineStr"/>
+      <c r="V162" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -12964,7 +13410,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T163" t="inlineStr"/>
-      <c r="U163" t="inlineStr">
+      <c r="U163" t="inlineStr"/>
+      <c r="V163" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13039,7 +13486,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T164" t="inlineStr"/>
-      <c r="U164" t="inlineStr">
+      <c r="U164" t="inlineStr"/>
+      <c r="V164" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13114,7 +13562,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T165" t="inlineStr"/>
-      <c r="U165" t="inlineStr">
+      <c r="U165" t="inlineStr"/>
+      <c r="V165" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13189,7 +13638,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T166" t="inlineStr"/>
-      <c r="U166" t="inlineStr">
+      <c r="U166" t="inlineStr"/>
+      <c r="V166" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13264,9 +13714,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T167" t="n">
-        <v>18.72514150278435</v>
-      </c>
-      <c r="U167" t="inlineStr">
+        <v>18.27792938213604</v>
+      </c>
+      <c r="U167" t="n">
+        <v>18.3463967312879</v>
+      </c>
+      <c r="V167" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -13341,7 +13794,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T168" t="inlineStr"/>
-      <c r="U168" t="inlineStr">
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13416,9 +13870,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T169" t="n">
-        <v>25.66336607697898</v>
-      </c>
-      <c r="U169" t="inlineStr">
+        <v>25.05044849958428</v>
+      </c>
+      <c r="U169" t="n">
+        <v>25.14428504791387</v>
+      </c>
+      <c r="V169" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -13493,7 +13950,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T170" t="inlineStr"/>
-      <c r="U170" t="inlineStr">
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13568,7 +14026,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T171" t="inlineStr"/>
-      <c r="U171" t="inlineStr">
+      <c r="U171" t="inlineStr"/>
+      <c r="V171" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13643,7 +14102,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T172" t="inlineStr"/>
-      <c r="U172" t="inlineStr">
+      <c r="U172" t="inlineStr"/>
+      <c r="V172" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13718,9 +14178,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T173" t="n">
-        <v>20.72879710116599</v>
-      </c>
-      <c r="U173" t="inlineStr">
+        <v>20.23373172028637</v>
+      </c>
+      <c r="U173" t="n">
+        <v>20.30952531513918</v>
+      </c>
+      <c r="V173" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -13795,7 +14258,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T174" t="inlineStr"/>
-      <c r="U174" t="inlineStr">
+      <c r="U174" t="inlineStr"/>
+      <c r="V174" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13870,7 +14334,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T175" t="inlineStr"/>
-      <c r="U175" t="inlineStr">
+      <c r="U175" t="inlineStr"/>
+      <c r="V175" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -13945,9 +14410,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T176" t="n">
-        <v>29.50987122758694</v>
-      </c>
-      <c r="U176" t="inlineStr">
+        <v>28.80508765680403</v>
+      </c>
+      <c r="U176" t="n">
+        <v>28.91298871893834</v>
+      </c>
+      <c r="V176" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14022,9 +14490,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T177" t="n">
-        <v>36.6961879814906</v>
-      </c>
-      <c r="U177" t="inlineStr">
+        <v>35.81977377418161</v>
+      </c>
+      <c r="U177" t="n">
+        <v>35.95395116956725</v>
+      </c>
+      <c r="V177" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14099,7 +14570,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T178" t="inlineStr"/>
-      <c r="U178" t="inlineStr">
+      <c r="U178" t="inlineStr"/>
+      <c r="V178" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -14174,7 +14646,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T179" t="inlineStr"/>
-      <c r="U179" t="inlineStr">
+      <c r="U179" t="inlineStr"/>
+      <c r="V179" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -14249,9 +14722,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T180" t="n">
-        <v>34.75777233444975</v>
-      </c>
-      <c r="U180" t="inlineStr">
+        <v>33.92765326312583</v>
+      </c>
+      <c r="U180" t="n">
+        <v>34.05474295875295</v>
+      </c>
+      <c r="V180" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14326,9 +14802,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T181" t="n">
-        <v>36.81721752698016</v>
-      </c>
-      <c r="U181" t="inlineStr">
+        <v>35.93791277384051</v>
+      </c>
+      <c r="U181" t="n">
+        <v>36.07253270645062</v>
+      </c>
+      <c r="V181" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14403,9 +14882,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T182" t="n">
-        <v>40.96445744820848</v>
-      </c>
-      <c r="U182" t="inlineStr">
+        <v>39.98610426012193</v>
+      </c>
+      <c r="U182" t="n">
+        <v>40.1358883250651</v>
+      </c>
+      <c r="V182" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14480,7 +14962,8 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T183" t="inlineStr"/>
-      <c r="U183" t="inlineStr">
+      <c r="U183" t="inlineStr"/>
+      <c r="V183" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -14555,9 +15038,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T184" t="n">
-        <v>27.65755095028403</v>
-      </c>
-      <c r="U184" t="inlineStr">
+        <v>26.99700630176557</v>
+      </c>
+      <c r="U184" t="n">
+        <v>27.09813446666178</v>
+      </c>
+      <c r="V184" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14632,9 +15118,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T185" t="n">
-        <v>24.35291569010893</v>
-      </c>
-      <c r="U185" t="inlineStr">
+        <v>23.77129556894063</v>
+      </c>
+      <c r="U185" t="n">
+        <v>23.86034053456466</v>
+      </c>
+      <c r="V185" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14709,9 +15198,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T186" t="n">
-        <v>31.84121364436432</v>
-      </c>
-      <c r="U186" t="inlineStr">
+        <v>31.08075067665886</v>
+      </c>
+      <c r="U186" t="n">
+        <v>31.1971761515576</v>
+      </c>
+      <c r="V186" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14786,9 +15278,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T187" t="n">
-        <v>27.09033845939206</v>
-      </c>
-      <c r="U187" t="inlineStr">
+        <v>26.44334053365124</v>
+      </c>
+      <c r="U187" t="n">
+        <v>26.54239472032669</v>
+      </c>
+      <c r="V187" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14863,9 +15358,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T188" t="n">
-        <v>26.85434647658429</v>
-      </c>
-      <c r="U188" t="inlineStr">
+        <v>26.2129847419009</v>
+      </c>
+      <c r="U188" t="n">
+        <v>26.31117603814205</v>
+      </c>
+      <c r="V188" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -14940,9 +15438,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T189" t="n">
-        <v>25.37199194564089</v>
-      </c>
-      <c r="U189" t="inlineStr">
+        <v>24.76603324987378</v>
+      </c>
+      <c r="U189" t="n">
+        <v>24.85880440628731</v>
+      </c>
+      <c r="V189" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -15017,9 +15518,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T190" t="n">
-        <v>25.69913381714493</v>
-      </c>
-      <c r="U190" t="inlineStr">
+        <v>25.08536199964059</v>
+      </c>
+      <c r="U190" t="n">
+        <v>25.17932933055219</v>
+      </c>
+      <c r="V190" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -15094,9 +15598,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T191" t="n">
-        <v>27.16742242664481</v>
-      </c>
-      <c r="U191" t="inlineStr">
+        <v>26.51858350630011</v>
+      </c>
+      <c r="U191" t="n">
+        <v>26.61791954584698</v>
+      </c>
+      <c r="V191" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -15171,9 +15678,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T192" t="n">
-        <v>28.13082497565271</v>
-      </c>
-      <c r="U192" t="inlineStr">
+        <v>27.45897713455216</v>
+      </c>
+      <c r="U192" t="n">
+        <v>27.56183579734259</v>
+      </c>
+      <c r="V192" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>
@@ -15248,9 +15758,12 @@
         <v>0.2942581907953586</v>
       </c>
       <c r="T193" t="n">
-        <v>19.9533022666929</v>
-      </c>
-      <c r="U193" t="inlineStr">
+        <v>19.47675801097673</v>
+      </c>
+      <c r="U193" t="n">
+        <v>19.54971605579701</v>
+      </c>
+      <c r="V193" t="inlineStr">
         <is>
           <t>1\carapace\car</t>
         </is>

</xml_diff>